<commit_message>
change h1 style add join button test to test doc
</commit_message>
<xml_diff>
--- a/assets/doc/test-cases.xlsx
+++ b/assets/doc/test-cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83ab32fafa566cfa/Full Stack Developer Training/project1_ccc/assets/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D22A09B-8733-494F-9387-2340238DA82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{6D22A09B-8733-494F-9387-2340238DA82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C9070C8-07B8-433B-9E57-2BF1673E8F37}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D07A67A7-5040-4BC6-8DB9-14DD9DC7A4A0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{D07A67A7-5040-4BC6-8DB9-14DD9DC7A4A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="24">
   <si>
     <t>Test Case</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>ü</t>
+  </si>
+  <si>
+    <t>navbar join us link opens in new tab</t>
+  </si>
+  <si>
+    <t>hero join us link opens in new tab</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9556E7-637F-4DE6-91D9-110EC2552685}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:E40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -633,14 +639,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>21</v>
@@ -655,171 +673,181 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>21</v>
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6" t="s">
+      <c r="D17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3" t="s">
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+      <c r="B21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="5" t="s">
-        <v>16</v>
+      <c r="D22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+      <c r="B26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
       </c>
@@ -828,8 +856,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="3" t="s">
-        <v>11</v>
+      <c r="A28" t="s">
+        <v>22</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>21</v>
@@ -846,7 +874,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>21</v>
@@ -856,25 +884,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>21</v>
+      <c r="A30" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>19</v>
+      <c r="A31" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>21</v>
@@ -889,20 +905,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="5" t="s">
-        <v>17</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>21</v>
@@ -913,57 +935,67 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
         <v>7</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>21</v>
@@ -974,7 +1006,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>21</v>
@@ -985,18 +1017,85 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="7" t="s">
+      <c r="B45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>